<commit_message>
add main and district
</commit_message>
<xml_diff>
--- a/src/main/resources/sample.xlsx
+++ b/src/main/resources/sample.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\five\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60CDA28-E9FE-4E08-A81D-489BEDC1CCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F321B4CC-62BC-42A7-9815-707DC6E30AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F8D5526-5AFA-44E1-B191-0008F3905F90}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>단체명</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -159,43 +159,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>다른것</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>900101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>여</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>테스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다른</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>데이터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>01033353331</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가입날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19900101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-01-01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -203,6 +179,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="yyyy&quot;/&quot;m&quot;/&quot;d;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -248,12 +227,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -567,301 +550,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F458F2-2721-499B-8984-280379A89450}">
-  <dimension ref="A1:R3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" style="1" bestFit="1"/>
-    <col min="2" max="2" width="11.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" bestFit="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="7" width="5.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.75" style="1" customWidth="1"/>
-    <col min="14" max="14" width="5.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" style="1" bestFit="1"/>
-    <col min="16" max="16" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="1" bestFit="1"/>
-    <col min="19" max="257" width="8.625" style="1"/>
-    <col min="258" max="259" width="8.375" style="1" customWidth="1"/>
-    <col min="260" max="513" width="8.625" style="1"/>
-    <col min="514" max="515" width="8.375" style="1" customWidth="1"/>
-    <col min="516" max="769" width="8.625" style="1"/>
-    <col min="770" max="771" width="8.375" style="1" customWidth="1"/>
-    <col min="772" max="1025" width="8.625" style="1"/>
-    <col min="1026" max="1027" width="8.375" style="1" customWidth="1"/>
-    <col min="1028" max="1281" width="8.625" style="1"/>
-    <col min="1282" max="1283" width="8.375" style="1" customWidth="1"/>
-    <col min="1284" max="1537" width="8.625" style="1"/>
-    <col min="1538" max="1539" width="8.375" style="1" customWidth="1"/>
-    <col min="1540" max="1793" width="8.625" style="1"/>
-    <col min="1794" max="1795" width="8.375" style="1" customWidth="1"/>
-    <col min="1796" max="2049" width="8.625" style="1"/>
-    <col min="2050" max="2051" width="8.375" style="1" customWidth="1"/>
-    <col min="2052" max="2305" width="8.625" style="1"/>
-    <col min="2306" max="2307" width="8.375" style="1" customWidth="1"/>
-    <col min="2308" max="2561" width="8.625" style="1"/>
-    <col min="2562" max="2563" width="8.375" style="1" customWidth="1"/>
-    <col min="2564" max="2817" width="8.625" style="1"/>
-    <col min="2818" max="2819" width="8.375" style="1" customWidth="1"/>
-    <col min="2820" max="3073" width="8.625" style="1"/>
-    <col min="3074" max="3075" width="8.375" style="1" customWidth="1"/>
-    <col min="3076" max="3329" width="8.625" style="1"/>
-    <col min="3330" max="3331" width="8.375" style="1" customWidth="1"/>
-    <col min="3332" max="3585" width="8.625" style="1"/>
-    <col min="3586" max="3587" width="8.375" style="1" customWidth="1"/>
-    <col min="3588" max="3841" width="8.625" style="1"/>
-    <col min="3842" max="3843" width="8.375" style="1" customWidth="1"/>
-    <col min="3844" max="4097" width="8.625" style="1"/>
-    <col min="4098" max="4099" width="8.375" style="1" customWidth="1"/>
-    <col min="4100" max="4353" width="8.625" style="1"/>
-    <col min="4354" max="4355" width="8.375" style="1" customWidth="1"/>
-    <col min="4356" max="4609" width="8.625" style="1"/>
-    <col min="4610" max="4611" width="8.375" style="1" customWidth="1"/>
-    <col min="4612" max="4865" width="8.625" style="1"/>
-    <col min="4866" max="4867" width="8.375" style="1" customWidth="1"/>
-    <col min="4868" max="5121" width="8.625" style="1"/>
-    <col min="5122" max="5123" width="8.375" style="1" customWidth="1"/>
-    <col min="5124" max="5377" width="8.625" style="1"/>
-    <col min="5378" max="5379" width="8.375" style="1" customWidth="1"/>
-    <col min="5380" max="5633" width="8.625" style="1"/>
-    <col min="5634" max="5635" width="8.375" style="1" customWidth="1"/>
-    <col min="5636" max="5889" width="8.625" style="1"/>
-    <col min="5890" max="5891" width="8.375" style="1" customWidth="1"/>
-    <col min="5892" max="6145" width="8.625" style="1"/>
-    <col min="6146" max="6147" width="8.375" style="1" customWidth="1"/>
-    <col min="6148" max="6401" width="8.625" style="1"/>
-    <col min="6402" max="6403" width="8.375" style="1" customWidth="1"/>
-    <col min="6404" max="6657" width="8.625" style="1"/>
-    <col min="6658" max="6659" width="8.375" style="1" customWidth="1"/>
-    <col min="6660" max="6913" width="8.625" style="1"/>
-    <col min="6914" max="6915" width="8.375" style="1" customWidth="1"/>
-    <col min="6916" max="7169" width="8.625" style="1"/>
-    <col min="7170" max="7171" width="8.375" style="1" customWidth="1"/>
-    <col min="7172" max="7425" width="8.625" style="1"/>
-    <col min="7426" max="7427" width="8.375" style="1" customWidth="1"/>
-    <col min="7428" max="7681" width="8.625" style="1"/>
-    <col min="7682" max="7683" width="8.375" style="1" customWidth="1"/>
-    <col min="7684" max="7937" width="8.625" style="1"/>
-    <col min="7938" max="7939" width="8.375" style="1" customWidth="1"/>
-    <col min="7940" max="8193" width="8.625" style="1"/>
-    <col min="8194" max="8195" width="8.375" style="1" customWidth="1"/>
-    <col min="8196" max="8449" width="8.625" style="1"/>
-    <col min="8450" max="8451" width="8.375" style="1" customWidth="1"/>
-    <col min="8452" max="8705" width="8.625" style="1"/>
-    <col min="8706" max="8707" width="8.375" style="1" customWidth="1"/>
-    <col min="8708" max="8961" width="8.625" style="1"/>
-    <col min="8962" max="8963" width="8.375" style="1" customWidth="1"/>
-    <col min="8964" max="9217" width="8.625" style="1"/>
-    <col min="9218" max="9219" width="8.375" style="1" customWidth="1"/>
-    <col min="9220" max="9473" width="8.625" style="1"/>
-    <col min="9474" max="9475" width="8.375" style="1" customWidth="1"/>
-    <col min="9476" max="9729" width="8.625" style="1"/>
-    <col min="9730" max="9731" width="8.375" style="1" customWidth="1"/>
-    <col min="9732" max="9985" width="8.625" style="1"/>
-    <col min="9986" max="9987" width="8.375" style="1" customWidth="1"/>
-    <col min="9988" max="10241" width="8.625" style="1"/>
-    <col min="10242" max="10243" width="8.375" style="1" customWidth="1"/>
-    <col min="10244" max="10497" width="8.625" style="1"/>
-    <col min="10498" max="10499" width="8.375" style="1" customWidth="1"/>
-    <col min="10500" max="10753" width="8.625" style="1"/>
-    <col min="10754" max="10755" width="8.375" style="1" customWidth="1"/>
-    <col min="10756" max="11009" width="8.625" style="1"/>
-    <col min="11010" max="11011" width="8.375" style="1" customWidth="1"/>
-    <col min="11012" max="11265" width="8.625" style="1"/>
-    <col min="11266" max="11267" width="8.375" style="1" customWidth="1"/>
-    <col min="11268" max="11521" width="8.625" style="1"/>
-    <col min="11522" max="11523" width="8.375" style="1" customWidth="1"/>
-    <col min="11524" max="11777" width="8.625" style="1"/>
-    <col min="11778" max="11779" width="8.375" style="1" customWidth="1"/>
-    <col min="11780" max="12033" width="8.625" style="1"/>
-    <col min="12034" max="12035" width="8.375" style="1" customWidth="1"/>
-    <col min="12036" max="12289" width="8.625" style="1"/>
-    <col min="12290" max="12291" width="8.375" style="1" customWidth="1"/>
-    <col min="12292" max="12545" width="8.625" style="1"/>
-    <col min="12546" max="12547" width="8.375" style="1" customWidth="1"/>
-    <col min="12548" max="12801" width="8.625" style="1"/>
-    <col min="12802" max="12803" width="8.375" style="1" customWidth="1"/>
-    <col min="12804" max="13057" width="8.625" style="1"/>
-    <col min="13058" max="13059" width="8.375" style="1" customWidth="1"/>
-    <col min="13060" max="13313" width="8.625" style="1"/>
-    <col min="13314" max="13315" width="8.375" style="1" customWidth="1"/>
-    <col min="13316" max="13569" width="8.625" style="1"/>
-    <col min="13570" max="13571" width="8.375" style="1" customWidth="1"/>
-    <col min="13572" max="13825" width="8.625" style="1"/>
-    <col min="13826" max="13827" width="8.375" style="1" customWidth="1"/>
-    <col min="13828" max="14081" width="8.625" style="1"/>
-    <col min="14082" max="14083" width="8.375" style="1" customWidth="1"/>
-    <col min="14084" max="14337" width="8.625" style="1"/>
-    <col min="14338" max="14339" width="8.375" style="1" customWidth="1"/>
-    <col min="14340" max="14593" width="8.625" style="1"/>
-    <col min="14594" max="14595" width="8.375" style="1" customWidth="1"/>
-    <col min="14596" max="14849" width="8.625" style="1"/>
-    <col min="14850" max="14851" width="8.375" style="1" customWidth="1"/>
-    <col min="14852" max="15105" width="8.625" style="1"/>
-    <col min="15106" max="15107" width="8.375" style="1" customWidth="1"/>
-    <col min="15108" max="15361" width="8.625" style="1"/>
-    <col min="15362" max="15363" width="8.375" style="1" customWidth="1"/>
-    <col min="15364" max="15617" width="8.625" style="1"/>
-    <col min="15618" max="15619" width="8.375" style="1" customWidth="1"/>
-    <col min="15620" max="15873" width="8.625" style="1"/>
-    <col min="15874" max="15875" width="8.375" style="1" customWidth="1"/>
-    <col min="15876" max="16129" width="8.625" style="1"/>
-    <col min="16130" max="16131" width="8.375" style="1" customWidth="1"/>
-    <col min="16132" max="16384" width="8.625" style="1"/>
+    <col min="6" max="6" width="8.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.75" style="1" customWidth="1"/>
+    <col min="13" max="13" width="5.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="1" bestFit="1"/>
+    <col min="15" max="15" width="8.75" style="1"/>
+    <col min="16" max="16" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="1" bestFit="1"/>
+    <col min="20" max="258" width="8.625" style="1"/>
+    <col min="259" max="260" width="8.375" style="1" customWidth="1"/>
+    <col min="261" max="514" width="8.625" style="1"/>
+    <col min="515" max="516" width="8.375" style="1" customWidth="1"/>
+    <col min="517" max="770" width="8.625" style="1"/>
+    <col min="771" max="772" width="8.375" style="1" customWidth="1"/>
+    <col min="773" max="1026" width="8.625" style="1"/>
+    <col min="1027" max="1028" width="8.375" style="1" customWidth="1"/>
+    <col min="1029" max="1282" width="8.625" style="1"/>
+    <col min="1283" max="1284" width="8.375" style="1" customWidth="1"/>
+    <col min="1285" max="1538" width="8.625" style="1"/>
+    <col min="1539" max="1540" width="8.375" style="1" customWidth="1"/>
+    <col min="1541" max="1794" width="8.625" style="1"/>
+    <col min="1795" max="1796" width="8.375" style="1" customWidth="1"/>
+    <col min="1797" max="2050" width="8.625" style="1"/>
+    <col min="2051" max="2052" width="8.375" style="1" customWidth="1"/>
+    <col min="2053" max="2306" width="8.625" style="1"/>
+    <col min="2307" max="2308" width="8.375" style="1" customWidth="1"/>
+    <col min="2309" max="2562" width="8.625" style="1"/>
+    <col min="2563" max="2564" width="8.375" style="1" customWidth="1"/>
+    <col min="2565" max="2818" width="8.625" style="1"/>
+    <col min="2819" max="2820" width="8.375" style="1" customWidth="1"/>
+    <col min="2821" max="3074" width="8.625" style="1"/>
+    <col min="3075" max="3076" width="8.375" style="1" customWidth="1"/>
+    <col min="3077" max="3330" width="8.625" style="1"/>
+    <col min="3331" max="3332" width="8.375" style="1" customWidth="1"/>
+    <col min="3333" max="3586" width="8.625" style="1"/>
+    <col min="3587" max="3588" width="8.375" style="1" customWidth="1"/>
+    <col min="3589" max="3842" width="8.625" style="1"/>
+    <col min="3843" max="3844" width="8.375" style="1" customWidth="1"/>
+    <col min="3845" max="4098" width="8.625" style="1"/>
+    <col min="4099" max="4100" width="8.375" style="1" customWidth="1"/>
+    <col min="4101" max="4354" width="8.625" style="1"/>
+    <col min="4355" max="4356" width="8.375" style="1" customWidth="1"/>
+    <col min="4357" max="4610" width="8.625" style="1"/>
+    <col min="4611" max="4612" width="8.375" style="1" customWidth="1"/>
+    <col min="4613" max="4866" width="8.625" style="1"/>
+    <col min="4867" max="4868" width="8.375" style="1" customWidth="1"/>
+    <col min="4869" max="5122" width="8.625" style="1"/>
+    <col min="5123" max="5124" width="8.375" style="1" customWidth="1"/>
+    <col min="5125" max="5378" width="8.625" style="1"/>
+    <col min="5379" max="5380" width="8.375" style="1" customWidth="1"/>
+    <col min="5381" max="5634" width="8.625" style="1"/>
+    <col min="5635" max="5636" width="8.375" style="1" customWidth="1"/>
+    <col min="5637" max="5890" width="8.625" style="1"/>
+    <col min="5891" max="5892" width="8.375" style="1" customWidth="1"/>
+    <col min="5893" max="6146" width="8.625" style="1"/>
+    <col min="6147" max="6148" width="8.375" style="1" customWidth="1"/>
+    <col min="6149" max="6402" width="8.625" style="1"/>
+    <col min="6403" max="6404" width="8.375" style="1" customWidth="1"/>
+    <col min="6405" max="6658" width="8.625" style="1"/>
+    <col min="6659" max="6660" width="8.375" style="1" customWidth="1"/>
+    <col min="6661" max="6914" width="8.625" style="1"/>
+    <col min="6915" max="6916" width="8.375" style="1" customWidth="1"/>
+    <col min="6917" max="7170" width="8.625" style="1"/>
+    <col min="7171" max="7172" width="8.375" style="1" customWidth="1"/>
+    <col min="7173" max="7426" width="8.625" style="1"/>
+    <col min="7427" max="7428" width="8.375" style="1" customWidth="1"/>
+    <col min="7429" max="7682" width="8.625" style="1"/>
+    <col min="7683" max="7684" width="8.375" style="1" customWidth="1"/>
+    <col min="7685" max="7938" width="8.625" style="1"/>
+    <col min="7939" max="7940" width="8.375" style="1" customWidth="1"/>
+    <col min="7941" max="8194" width="8.625" style="1"/>
+    <col min="8195" max="8196" width="8.375" style="1" customWidth="1"/>
+    <col min="8197" max="8450" width="8.625" style="1"/>
+    <col min="8451" max="8452" width="8.375" style="1" customWidth="1"/>
+    <col min="8453" max="8706" width="8.625" style="1"/>
+    <col min="8707" max="8708" width="8.375" style="1" customWidth="1"/>
+    <col min="8709" max="8962" width="8.625" style="1"/>
+    <col min="8963" max="8964" width="8.375" style="1" customWidth="1"/>
+    <col min="8965" max="9218" width="8.625" style="1"/>
+    <col min="9219" max="9220" width="8.375" style="1" customWidth="1"/>
+    <col min="9221" max="9474" width="8.625" style="1"/>
+    <col min="9475" max="9476" width="8.375" style="1" customWidth="1"/>
+    <col min="9477" max="9730" width="8.625" style="1"/>
+    <col min="9731" max="9732" width="8.375" style="1" customWidth="1"/>
+    <col min="9733" max="9986" width="8.625" style="1"/>
+    <col min="9987" max="9988" width="8.375" style="1" customWidth="1"/>
+    <col min="9989" max="10242" width="8.625" style="1"/>
+    <col min="10243" max="10244" width="8.375" style="1" customWidth="1"/>
+    <col min="10245" max="10498" width="8.625" style="1"/>
+    <col min="10499" max="10500" width="8.375" style="1" customWidth="1"/>
+    <col min="10501" max="10754" width="8.625" style="1"/>
+    <col min="10755" max="10756" width="8.375" style="1" customWidth="1"/>
+    <col min="10757" max="11010" width="8.625" style="1"/>
+    <col min="11011" max="11012" width="8.375" style="1" customWidth="1"/>
+    <col min="11013" max="11266" width="8.625" style="1"/>
+    <col min="11267" max="11268" width="8.375" style="1" customWidth="1"/>
+    <col min="11269" max="11522" width="8.625" style="1"/>
+    <col min="11523" max="11524" width="8.375" style="1" customWidth="1"/>
+    <col min="11525" max="11778" width="8.625" style="1"/>
+    <col min="11779" max="11780" width="8.375" style="1" customWidth="1"/>
+    <col min="11781" max="12034" width="8.625" style="1"/>
+    <col min="12035" max="12036" width="8.375" style="1" customWidth="1"/>
+    <col min="12037" max="12290" width="8.625" style="1"/>
+    <col min="12291" max="12292" width="8.375" style="1" customWidth="1"/>
+    <col min="12293" max="12546" width="8.625" style="1"/>
+    <col min="12547" max="12548" width="8.375" style="1" customWidth="1"/>
+    <col min="12549" max="12802" width="8.625" style="1"/>
+    <col min="12803" max="12804" width="8.375" style="1" customWidth="1"/>
+    <col min="12805" max="13058" width="8.625" style="1"/>
+    <col min="13059" max="13060" width="8.375" style="1" customWidth="1"/>
+    <col min="13061" max="13314" width="8.625" style="1"/>
+    <col min="13315" max="13316" width="8.375" style="1" customWidth="1"/>
+    <col min="13317" max="13570" width="8.625" style="1"/>
+    <col min="13571" max="13572" width="8.375" style="1" customWidth="1"/>
+    <col min="13573" max="13826" width="8.625" style="1"/>
+    <col min="13827" max="13828" width="8.375" style="1" customWidth="1"/>
+    <col min="13829" max="14082" width="8.625" style="1"/>
+    <col min="14083" max="14084" width="8.375" style="1" customWidth="1"/>
+    <col min="14085" max="14338" width="8.625" style="1"/>
+    <col min="14339" max="14340" width="8.375" style="1" customWidth="1"/>
+    <col min="14341" max="14594" width="8.625" style="1"/>
+    <col min="14595" max="14596" width="8.375" style="1" customWidth="1"/>
+    <col min="14597" max="14850" width="8.625" style="1"/>
+    <col min="14851" max="14852" width="8.375" style="1" customWidth="1"/>
+    <col min="14853" max="15106" width="8.625" style="1"/>
+    <col min="15107" max="15108" width="8.375" style="1" customWidth="1"/>
+    <col min="15109" max="15362" width="8.625" style="1"/>
+    <col min="15363" max="15364" width="8.375" style="1" customWidth="1"/>
+    <col min="15365" max="15618" width="8.625" style="1"/>
+    <col min="15619" max="15620" width="8.375" style="1" customWidth="1"/>
+    <col min="15621" max="15874" width="8.625" style="1"/>
+    <col min="15875" max="15876" width="8.375" style="1" customWidth="1"/>
+    <col min="15877" max="16130" width="8.625" style="1"/>
+    <col min="16131" max="16132" width="8.375" style="1" customWidth="1"/>
+    <col min="16133" max="16383" width="8.625" style="1"/>
+    <col min="16384" max="16384" width="8.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>